<commit_message>
Actualización de los planes individuales
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20095495.xlsx
+++ b/tspi/ciclo-4/plan4-20095495.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>Cada miembro del equipo completó la forma PEER. Se creó el reporte del ciclo correspondiente. Se completaron las formas SUMP y SUMQ para el sistema y todos sus componentes.</t>
+  </si>
+  <si>
+    <t>El equipo ha completado los productos especificados. El equipo ha acumulado toda la información y ha completado todas las formas requeridas.</t>
+  </si>
+  <si>
+    <t>Se ha implementado la funcionalidad #3 del producto.</t>
+  </si>
+  <si>
+    <t>El equipo ha completado un ciclo preeviamente.</t>
+  </si>
+  <si>
+    <t>El equipo ha completado un ciclo preeviamente. Cada miembro del equipo ha leído el capítulo correspondiente a su rol.</t>
+  </si>
+  <si>
+    <t>Se ha completado la reunión de equipo para analizar la versión final del documento de requerimientos. Se ha creado el esquema del documento de arquitectura.</t>
   </si>
 </sst>
 </file>
@@ -665,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -725,7 +740,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>21</v>
@@ -1762,7 +1777,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>23</v>
@@ -2799,7 +2814,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>25</v>
@@ -3835,9 +3850,7 @@
       <c r="B5" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>27</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="30" t="s">
         <v>27</v>
       </c>
@@ -4873,7 +4886,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>29</v>
@@ -4907,9 +4920,7 @@
       <c r="B7" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>31</v>
-      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="30" t="s">
         <v>31</v>
       </c>
@@ -4943,7 +4954,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Actualizacion de las graficas generales del plan del proyecto
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20095495.xlsx
+++ b/tspi/ciclo-4/plan4-20095495.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\github\PPR\tspi\ciclo-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\github\ppr\tspi\ciclo-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
Actualizando lo del dia de hoy
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20095495.xlsx
+++ b/tspi/ciclo-4/plan4-20095495.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\github\ppr\tspi\ciclo-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="1"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Creando la vista de descomposicion</t>
+  </si>
+  <si>
+    <t>Inspeccionando lo nuevo agregado por Hector en las vistas y viendo como conectarlo con el controlador</t>
+  </si>
+  <si>
+    <t>Tutorial avanzado de Rails</t>
+  </si>
+  <si>
+    <t>Agregando el controlador encargado de salvar  el horario de un usuario en la base de datos</t>
   </si>
 </sst>
 </file>
@@ -714,7 +723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALY9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5030,7 +5041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5159,8 +5170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5255,22 +5266,86 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="18"/>
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <v>41966</v>
+      </c>
+      <c r="B4" s="17">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.4680555555555555</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" ref="F4" si="1">((HOUR(D4)-HOUR(C4))*60)+(MINUTE(D4)-MINUTE(C4))-E4</f>
+        <v>72</v>
+      </c>
+      <c r="G4" s="17">
+        <v>70</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
+        <v>41966</v>
+      </c>
+      <c r="B5" s="17">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F6" si="2">((HOUR(D5)-HOUR(C5))*60)+(MINUTE(D5)-MINUTE(C5))-E5</f>
+        <v>102</v>
+      </c>
+      <c r="G5" s="17">
+        <v>70</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>41966</v>
+      </c>
+      <c r="B6" s="17">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="G6" s="17">
+        <v>70</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>

</xml_diff>

<commit_message>
Actualizando vista de decomposition
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20095495.xlsx
+++ b/tspi/ciclo-4/plan4-20095495.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Id</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Agregando el controlador encargado de salvar  el horario de un usuario en la base de datos</t>
+  </si>
+  <si>
+    <t>Reunion con Alan y Hector</t>
+  </si>
+  <si>
+    <t>Actualizando la vista de descomposicion</t>
   </si>
 </sst>
 </file>
@@ -5082,7 +5088,7 @@
       </c>
       <c r="B3" s="4">
         <f>SUMIF(logt!G:G,task!A3,logt!F:F)/60</f>
-        <v>1.6333333333333333</v>
+        <v>1.7666666666666666</v>
       </c>
       <c r="C3" s="4">
         <v>9</v>
@@ -5171,7 +5177,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5348,19 +5354,58 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="18"/>
-      <c r="H7" s="8"/>
+      <c r="A7" s="19">
+        <v>41967</v>
+      </c>
+      <c r="B7" s="17">
+        <v>8</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.90555555555555556</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" ref="F7" si="3">((HOUR(D7)-HOUR(C7))*60)+(MINUTE(D7)-MINUTE(C7))-E7</f>
+        <v>10</v>
+      </c>
+      <c r="G7" s="17">
+        <v>76</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="18"/>
+      <c r="A8" s="19">
+        <v>41967</v>
+      </c>
+      <c r="B8" s="17">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" ref="F8" si="4">((HOUR(D8)-HOUR(C8))*60)+(MINUTE(D8)-MINUTE(C8))-E8</f>
+        <v>8</v>
+      </c>
+      <c r="G8" s="17">
+        <v>65</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>

</xml_diff>

<commit_message>
Actualizando el dia de ayer
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20095495.xlsx
+++ b/tspi/ciclo-4/plan4-20095495.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\PPR\tspi\ciclo-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gogi\Documents\GitHub\ppr\tspi\ciclo-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Actualizando la vista de descomposicion</t>
+  </si>
+  <si>
+    <t>Ayudando a Hector con un problema de AJAX</t>
   </si>
 </sst>
 </file>
@@ -5177,7 +5180,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5408,11 +5411,31 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="19">
+        <v>41967</v>
+      </c>
+      <c r="B9" s="17">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.97152777777777777</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" ref="F9" si="5">((HOUR(D9)-HOUR(C9))*60)+(MINUTE(D9)-MINUTE(C9))-E9</f>
+        <v>55</v>
+      </c>
+      <c r="G9" s="17">
+        <v>70</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="24"/>

</xml_diff>